<commit_message>
new file:   ontology/cataldo/igso-clouddomain.rdf 	new file:   ontology/cataldo/igso-properties.ttl 	modified:   ontology/cataldo/igsoMatuLevelv1.2.ttl 	modified:   ontology/cataldo/igsoProperties.xlsx
</commit_message>
<xml_diff>
--- a/ontology/cataldo/igsoProperties.xlsx
+++ b/ontology/cataldo/igsoProperties.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="19200" windowHeight="7040" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="19200" windowHeight="7040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
     <sheet name="igsoProperties" sheetId="1" r:id="rId2"/>
     <sheet name="RegulatorySchema" sheetId="3" r:id="rId3"/>
+    <sheet name="Regulations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="igsoProperties" localSheetId="0">Tabelle1!$A$1:$GS$1010</definedName>
@@ -236,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="2486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4182" uniqueCount="2512">
   <si>
     <t>Entity,Type,Superclass(es),ensure_fair_processing,validate_authenticity,submitts,has_half-life,'is_tagging_of -&gt; data',has_cost,delends_on,defines_design_of,impact_assessments,ensure_accountability,implements,has_importance,validate_provenance,has_price,is_easy_to_collect,requires,minize_amount,is_easy_to_digitize,capture_records_of,classify_as,enforces_governance_of,defines_desirable,is_categorized_by,referential_integrity,to_notify,uses,ensure_accuracy,is_classified_by,discloses,provides_relational_search_service,ensures_referential_integrity,mandates,is_collected_by,is_compliant_with,provides_database_service,has_value,is_composed_of,'is_taxonomy_of -&gt;  ML, AI',requires_compliance_with,is_secured_by,data_transfer,provides_referential_integrity,is_metadata_of,ensure_transparancy,being_notified,provides_fulltext_service,is_stored_in,'is managed by',ensure_integrity,has_capability,provides_index_service,monitors,consists_of,provides,ensure_lawfulness_processing,is_an_expense,has_obligations,limit_storage_period,is,designs,is_administered_by,specifies,has,'is_governed_by an IGProgram,',Classify,is_classiffied_by,is_retrieved,cooperation_with,is_specified_by,has_member,complies_with,be_appointed,requires_referential_integrity,comply_with_,is_searched_using,implements_relational_index_service,plan,is_governd_by,is_disposed_by,is_member_of,is_defined_by,handles,provides_fulltext_search_service,implements_fulltext_service,implements_database_service,is_responsible_for,requires_design_of,is_archived,provides_relational_index_service,implements_relational_search_service,avoids_orphan_contentobjects,is_hard_to,requires_twophase_commit_protocol,provides_catalog_service,limit_purpose,avoids_dangling_pointers,developes,provides_search_service,complies,provides_fulltext_index_service,is_obligated_to_esure,has_risk,has_maturity_level,align,analyze,appoint,approve,aquire,archive,assess,audit,backup,build,classify,communicate,conduct_inventory,control,convert,coordinate,correct,create,defines,defines_maturity,design,develop,distribute,ensure,establish,estimate,evaluate,governs,has_maturity,manage,measure,monitor,produces,profile,promote,test,validate,owl:topObjectProperty,risk,value,maturitylevel,cost,owl:topDataProperty,abstract,contributor,creator,description,issued,license,modified,publisher,references,rights,source,title,igso:isReferencedBy,contentLanguage,copyright,fileAbbreviation,fileAbstract,filename,relatedSpecification,rdfs:comment,rdfs:isDefinedBy,rdfs:label,'alternative label','change note',definition,'editorial note',example,skos:historyNote,note,'preferred label','scope note','construct regex','parse regex','actual expression','common designation','definition origin','has maturity level','preferred designation','term origin',abbreviation,acronym,'adapted from',copyright,'direct source','explanatory note','logical definition',symbol,synonym,'usage note',</t>
   </si>
@@ -7695,6 +7696,84 @@
   </si>
   <si>
     <t>Articles</t>
+  </si>
+  <si>
+    <t>Rights of Data Subjects:</t>
+  </si>
+  <si>
+    <t>Right to be informed</t>
+  </si>
+  <si>
+    <t>Right of access</t>
+  </si>
+  <si>
+    <t>Right to rectification</t>
+  </si>
+  <si>
+    <t>Right to erasure (right to be forgotten)</t>
+  </si>
+  <si>
+    <t>Right to restrict processing</t>
+  </si>
+  <si>
+    <t>Right to data portability</t>
+  </si>
+  <si>
+    <t>Right to object</t>
+  </si>
+  <si>
+    <t>Rights related to automated decision-making and profiling</t>
+  </si>
+  <si>
+    <t>Obligations of DataControllers and DataProcessors:</t>
+  </si>
+  <si>
+    <t>Lawfulness, fairness, and transparency of data processing</t>
+  </si>
+  <si>
+    <t>Purpose limitation</t>
+  </si>
+  <si>
+    <t>Data minimization</t>
+  </si>
+  <si>
+    <t>Accuracy of data</t>
+  </si>
+  <si>
+    <t>Storage limitation</t>
+  </si>
+  <si>
+    <t>Integrity and confidentiality of data</t>
+  </si>
+  <si>
+    <t>Accountability of data controllers and processors</t>
+  </si>
+  <si>
+    <t>Data protection impact assessments</t>
+  </si>
+  <si>
+    <t>Data protection officers</t>
+  </si>
+  <si>
+    <t>Notification of personal data breaches</t>
+  </si>
+  <si>
+    <t>Cooperation with supervisory authorities</t>
+  </si>
+  <si>
+    <t>Cross-border data transfers</t>
+  </si>
+  <si>
+    <t>Records of processing activities</t>
+  </si>
+  <si>
+    <t>Consent requirements</t>
+  </si>
+  <si>
+    <t>Restrictions</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
   </si>
 </sst>
 </file>
@@ -8178,7 +8257,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -8186,6 +8265,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -20274,7 +20356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1010"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -25185,7 +25267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -25198,20 +25280,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>1800</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="3" t="s">
         <v>2473</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2474</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>2475</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="2" t="s">
         <v>2478</v>
       </c>
@@ -25258,4 +25340,220 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.6328125" customWidth="1"/>
+    <col min="2" max="2" width="49.08984375" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="49.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2510</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C6">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" ref="A7:A12" si="0">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2489</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C18" si="1">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2491</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   064.rdf 	modified:   catalog-v001.xml 	new file:   cmOrganization.ttl 	new file:   cmOrganizationv1.0.ttl 	new file:   dcat-new.ttl 	new file:   goodrelationv1.owl 	modified:   igsOrgStruct.txt 	new file:   igsOrgStruct.txt - Shortcut.lnk 	modified:   igso-mlv1.2.rdf 	new file:   igso-org.ttl 	modified:   igsoMatuLevelv1.2.ttl 	modified:   igsoProperties.xlsx 	new file:   igsoPropertiesExport.csv 	new file:   myorg.ttl 	new file:   org.rdf 	new file:   org.ttl 	new file:   prov-o-20130430.rdf 	new file:   w3org.ttl
</commit_message>
<xml_diff>
--- a/ontology/cataldo/igsoProperties.xlsx
+++ b/ontology/cataldo/igsoProperties.xlsx
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4182" uniqueCount="2512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="2526">
   <si>
     <t>Entity,Type,Superclass(es),ensure_fair_processing,validate_authenticity,submitts,has_half-life,'is_tagging_of -&gt; data',has_cost,delends_on,defines_design_of,impact_assessments,ensure_accountability,implements,has_importance,validate_provenance,has_price,is_easy_to_collect,requires,minize_amount,is_easy_to_digitize,capture_records_of,classify_as,enforces_governance_of,defines_desirable,is_categorized_by,referential_integrity,to_notify,uses,ensure_accuracy,is_classified_by,discloses,provides_relational_search_service,ensures_referential_integrity,mandates,is_collected_by,is_compliant_with,provides_database_service,has_value,is_composed_of,'is_taxonomy_of -&gt;  ML, AI',requires_compliance_with,is_secured_by,data_transfer,provides_referential_integrity,is_metadata_of,ensure_transparancy,being_notified,provides_fulltext_service,is_stored_in,'is managed by',ensure_integrity,has_capability,provides_index_service,monitors,consists_of,provides,ensure_lawfulness_processing,is_an_expense,has_obligations,limit_storage_period,is,designs,is_administered_by,specifies,has,'is_governed_by an IGProgram,',Classify,is_classiffied_by,is_retrieved,cooperation_with,is_specified_by,has_member,complies_with,be_appointed,requires_referential_integrity,comply_with_,is_searched_using,implements_relational_index_service,plan,is_governd_by,is_disposed_by,is_member_of,is_defined_by,handles,provides_fulltext_search_service,implements_fulltext_service,implements_database_service,is_responsible_for,requires_design_of,is_archived,provides_relational_index_service,implements_relational_search_service,avoids_orphan_contentobjects,is_hard_to,requires_twophase_commit_protocol,provides_catalog_service,limit_purpose,avoids_dangling_pointers,developes,provides_search_service,complies,provides_fulltext_index_service,is_obligated_to_esure,has_risk,has_maturity_level,align,analyze,appoint,approve,aquire,archive,assess,audit,backup,build,classify,communicate,conduct_inventory,control,convert,coordinate,correct,create,defines,defines_maturity,design,develop,distribute,ensure,establish,estimate,evaluate,governs,has_maturity,manage,measure,monitor,produces,profile,promote,test,validate,owl:topObjectProperty,risk,value,maturitylevel,cost,owl:topDataProperty,abstract,contributor,creator,description,issued,license,modified,publisher,references,rights,source,title,igso:isReferencedBy,contentLanguage,copyright,fileAbbreviation,fileAbstract,filename,relatedSpecification,rdfs:comment,rdfs:isDefinedBy,rdfs:label,'alternative label','change note',definition,'editorial note',example,skos:historyNote,note,'preferred label','scope note','construct regex','parse regex','actual expression','common designation','definition origin','has maturity level','preferred designation','term origin',abbreviation,acronym,'adapted from',copyright,'direct source','explanatory note','logical definition',symbol,synonym,'usage note',</t>
   </si>
@@ -7722,12 +7722,6 @@
     <t>Right to object</t>
   </si>
   <si>
-    <t>Rights related to automated decision-making and profiling</t>
-  </si>
-  <si>
-    <t>Obligations of DataControllers and DataProcessors:</t>
-  </si>
-  <si>
     <t>Lawfulness, fairness, and transparency of data processing</t>
   </si>
   <si>
@@ -7752,9 +7746,6 @@
     <t>Data protection impact assessments</t>
   </si>
   <si>
-    <t>Data protection officers</t>
-  </si>
-  <si>
     <t>Notification of personal data breaches</t>
   </si>
   <si>
@@ -7764,16 +7755,69 @@
     <t>Cross-border data transfers</t>
   </si>
   <si>
-    <t>Records of processing activities</t>
-  </si>
-  <si>
     <t>Consent requirements</t>
   </si>
   <si>
-    <t>Restrictions</t>
-  </si>
-  <si>
     <t>Exceptions</t>
+  </si>
+  <si>
+    <t>Right related to automated decision-making</t>
+  </si>
+  <si>
+    <t>Right related to automated profiling</t>
+  </si>
+  <si>
+    <t>Right to be forgotten</t>
+  </si>
+  <si>
+    <t>Capture records of data processing activities</t>
+  </si>
+  <si>
+    <t>Appoint DataProtectionOfficer</t>
+  </si>
+  <si>
+    <t>Derived 
+Funtional &amp; Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>Obligations of 
+DataControllers and DataProcessors:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataOwnerProfile,CustomerDataBase, RDBMS, ComunicationMethod, </t>
+  </si>
+  <si>
+    <t>UserPortal, AccessAPI,InformationRetieval, Search, Query, Store, Retrieve, Transfer</t>
+  </si>
+  <si>
+    <t>Administration, Management, Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security, Privacy, Records, Case, </t>
+  </si>
+  <si>
+    <t>eDiscovery, Retrive, Transfer</t>
+  </si>
+  <si>
+    <t>CaseManagement</t>
+  </si>
+  <si>
+    <t>ContentRepository, Retention, Disposition, Schedules, Classification, Hold, Policies, Rules</t>
+  </si>
+  <si>
+    <t>Monitoring, Records, Workflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deletion, Disposal, </t>
+  </si>
+  <si>
+    <t>Classification. Policies, Rules, Control, Monitoring, RecordsManagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repository, </t>
+  </si>
+  <si>
+    <t>Role, Responsibility</t>
   </si>
 </sst>
 </file>
@@ -8257,7 +8301,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -8270,6 +8314,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -25268,7 +25327,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25344,215 +25403,308 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:F18"/>
+  <dimension ref="A4:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.6328125" customWidth="1"/>
-    <col min="2" max="2" width="49.08984375" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="49.6328125" customWidth="1"/>
+    <col min="2" max="2" width="39.36328125" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" customWidth="1"/>
+    <col min="6" max="6" width="34.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>2486</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>2495</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>2510</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>2511</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C4" s="3" t="s">
+        <v>2512</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2513</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2512</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>2487</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>2496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="E5" s="7" t="s">
+        <v>2494</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>2523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>2488</v>
       </c>
-      <c r="C6">
-        <f>C5+1</f>
+      <c r="C6" s="7" t="s">
+        <v>2515</v>
+      </c>
+      <c r="D6">
+        <f>D5+1</f>
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>2497</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <f t="shared" ref="A7:A12" si="0">A6+1</f>
+      <c r="E6" s="7" t="s">
+        <v>2495</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <f t="shared" ref="A7:A15" si="0">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>2489</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C18" si="1">C6+1</f>
+      <c r="C7" s="8" t="s">
+        <v>2516</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D18" si="1">D6+1</f>
         <v>3</v>
       </c>
-      <c r="D7" t="s">
-        <v>2498</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="E7" s="7" t="s">
+        <v>2496</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>2490</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7" t="s">
+        <v>2520</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>2499</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="E8" s="7" t="s">
+        <v>2497</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>2491</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D9" t="s">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="E9" s="7" t="s">
+        <v>2498</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>2492</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7" t="s">
+        <v>2518</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D10" t="s">
-        <v>2501</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="E10" s="7" t="s">
+        <v>2499</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>2493</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>2502</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="E11" s="7" t="s">
+        <v>2500</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>2494</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="7" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>2521</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>2503</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C13">
+      <c r="E12" s="7" t="s">
+        <v>2501</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>2508</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D13" t="s">
-        <v>2504</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C14">
+      <c r="E13" s="7" t="s">
+        <v>2511</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>2525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2522</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D14" t="s">
-        <v>2505</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C15">
+      <c r="E14" s="7" t="s">
+        <v>2502</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D15" t="s">
-        <v>2506</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C16">
+      <c r="E15" s="7" t="s">
+        <v>2503</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
+      <c r="D16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D16" t="s">
-        <v>2507</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C17">
+      <c r="E16" s="7" t="s">
+        <v>2504</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="3:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="C17" s="6"/>
+      <c r="D17">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D17" t="s">
-        <v>2508</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C18">
+      <c r="E17" s="7" t="s">
+        <v>2510</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C18" s="6"/>
+      <c r="D18">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="D18" t="s">
-        <v>2509</v>
-      </c>
+      <c r="E18" s="7" t="s">
+        <v>2505</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C19" s="6"/>
+      <c r="E19" s="7" t="s">
+        <v>2496</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C20" s="6"/>
+      <c r="E20" s="7" t="s">
+        <v>2511</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>